<commit_message>
Solved reactance lines problem
</commit_message>
<xml_diff>
--- a/test/configs/data/develop/pypsa-it_capacity_expansion.xlsx
+++ b/test/configs/data/develop/pypsa-it_capacity_expansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="1" r:id="rId1"/>
@@ -1718,7 +1718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -3268,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="N2" t="e">
-        <f>-inf</f>
+        <f t="shared" ref="N2:N49" si="0">-inf</f>
         <v>#NAME?</v>
       </c>
       <c r="O2" t="s">
@@ -3373,7 +3373,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O3" t="s">
@@ -3478,7 +3478,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O4" t="s">
@@ -3583,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O5" t="s">
@@ -3688,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O6" t="s">
@@ -3793,7 +3793,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O7" t="s">
@@ -3898,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O8" t="s">
@@ -4003,7 +4003,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O9" t="s">
@@ -4108,7 +4108,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O10" t="s">
@@ -4213,7 +4213,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O11" t="s">
@@ -4318,7 +4318,7 @@
         <v>1</v>
       </c>
       <c r="N12" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O12" t="s">
@@ -4423,7 +4423,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O13" t="s">
@@ -4528,7 +4528,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O14" t="s">
@@ -4633,7 +4633,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O15" t="s">
@@ -4738,7 +4738,7 @@
         <v>1</v>
       </c>
       <c r="N16" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O16" t="s">
@@ -4843,7 +4843,7 @@
         <v>1</v>
       </c>
       <c r="N17" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O17" t="s">
@@ -4948,7 +4948,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O18" t="s">
@@ -5053,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="N19" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O19" t="s">
@@ -5158,7 +5158,7 @@
         <v>1</v>
       </c>
       <c r="N20" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O20" t="s">
@@ -5263,7 +5263,7 @@
         <v>1</v>
       </c>
       <c r="N21" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O21" t="s">
@@ -5368,7 +5368,7 @@
         <v>1</v>
       </c>
       <c r="N22" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O22" t="s">
@@ -5473,7 +5473,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O23" t="s">
@@ -5578,7 +5578,7 @@
         <v>1</v>
       </c>
       <c r="N24" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O24" t="s">
@@ -5683,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="N25" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O25" t="s">
@@ -5788,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="N26" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O26" t="s">
@@ -5893,7 +5893,7 @@
         <v>1</v>
       </c>
       <c r="N27" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O27" t="s">
@@ -5998,7 +5998,7 @@
         <v>1</v>
       </c>
       <c r="N28" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O28" t="s">
@@ -6103,7 +6103,7 @@
         <v>1</v>
       </c>
       <c r="N29" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O29" t="s">
@@ -6208,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="N30" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O30" t="s">
@@ -6313,7 +6313,7 @@
         <v>1</v>
       </c>
       <c r="N31" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O31" t="s">
@@ -6418,7 +6418,7 @@
         <v>1</v>
       </c>
       <c r="N32" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O32" t="s">
@@ -6523,7 +6523,7 @@
         <v>1</v>
       </c>
       <c r="N33" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O33" t="s">
@@ -6628,7 +6628,7 @@
         <v>1</v>
       </c>
       <c r="N34" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O34" t="s">
@@ -6733,7 +6733,7 @@
         <v>1</v>
       </c>
       <c r="N35" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O35" t="s">
@@ -6838,7 +6838,7 @@
         <v>1</v>
       </c>
       <c r="N36" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O36" t="s">
@@ -6943,7 +6943,7 @@
         <v>1</v>
       </c>
       <c r="N37" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O37" t="s">
@@ -7048,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="N38" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O38" t="s">
@@ -7153,7 +7153,7 @@
         <v>1</v>
       </c>
       <c r="N39" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O39" t="s">
@@ -7258,7 +7258,7 @@
         <v>1</v>
       </c>
       <c r="N40" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O40" t="s">
@@ -7363,7 +7363,7 @@
         <v>1</v>
       </c>
       <c r="N41" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O41" t="s">
@@ -7468,7 +7468,7 @@
         <v>1</v>
       </c>
       <c r="N42" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O42" t="s">
@@ -7573,7 +7573,7 @@
         <v>1</v>
       </c>
       <c r="N43" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O43" t="s">
@@ -7678,7 +7678,7 @@
         <v>1</v>
       </c>
       <c r="N44" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O44" t="s">
@@ -7783,7 +7783,7 @@
         <v>1</v>
       </c>
       <c r="N45" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O45" t="s">
@@ -7888,7 +7888,7 @@
         <v>1</v>
       </c>
       <c r="N46" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O46" t="s">
@@ -7993,7 +7993,7 @@
         <v>1</v>
       </c>
       <c r="N47" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O47" t="s">
@@ -8098,7 +8098,7 @@
         <v>1</v>
       </c>
       <c r="N48" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O48" t="s">
@@ -8203,7 +8203,7 @@
         <v>1</v>
       </c>
       <c r="N49" t="e">
-        <f>-inf</f>
+        <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
       <c r="O49" t="s">
@@ -11885,7 +11885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>